<commit_message>
Added more explanation to linear regression example
</commit_message>
<xml_diff>
--- a/Part 2 - Regression/Section 4 - Simple Linear Regression/NET/Dataset/Sprint_Data.xlsx
+++ b/Part 2 - Regression/Section 4 - Simple Linear Regression/NET/Dataset/Sprint_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\Machine learning\Machine Learning A-Z\Part 2 - Regression\Section 4 - Simple Linear Regression\NET\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F53EFD0F-C3F4-4E94-8CC1-CB17AF50AB24}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FFC2B418-D34F-4A13-8A41-BEF101FD7CC0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -759,31 +759,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="199"/>
                 <c:pt idx="0">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>198</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>164</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>129</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>85</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>82</c:v>
+                  <c:v>153</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>145</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>196</c:v>
+                  <c:v>198</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>193</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>122</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -795,31 +795,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="199"/>
                 <c:pt idx="0">
-                  <c:v>155.4</c:v>
+                  <c:v>129.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>127.20000000000002</c:v>
+                  <c:v>111.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>108.2</c:v>
+                  <c:v>94.800000000000011</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>63</c:v>
+                  <c:v>153.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57.600000000000009</c:v>
+                  <c:v>125.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>124</c:v>
+                  <c:v>126.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>151.80000000000001</c:v>
+                  <c:v>163.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>152.4</c:v>
+                  <c:v>48.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>94.600000000000009</c:v>
+                  <c:v>106.60000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1619,7 +1619,7 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>22828</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1437573" cy="358560"/>
+    <xdr:ext cx="1565108" cy="358560"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
@@ -1636,7 +1636,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="9941750" y="3832828"/>
-              <a:ext cx="1437573" cy="358560"/>
+              <a:ext cx="1565108" cy="358560"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1663,6 +1663,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1744,7 +1745,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1756,7 +1757,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1771,7 +1772,7 @@
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
                                         <a:effectLst/>
-                                        <a:latin typeface="+mn-lt"/>
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:ea typeface="+mn-ea"/>
                                         <a:cs typeface="+mn-cs"/>
                                       </a:rPr>
@@ -1784,7 +1785,7 @@
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
                                         <a:effectLst/>
-                                        <a:latin typeface="+mn-lt"/>
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:ea typeface="+mn-ea"/>
                                         <a:cs typeface="+mn-cs"/>
                                       </a:rPr>
@@ -1804,7 +1805,7 @@
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
-                              <m:t> (</m:t>
+                              <m:t> ∗(</m:t>
                             </m:r>
                             <m:r>
                               <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
@@ -1959,7 +1960,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="9941750" y="3832828"/>
-              <a:ext cx="1437573" cy="358560"/>
+              <a:ext cx="1565108" cy="358560"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1986,6 +1987,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="nl-NL" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -2002,7 +2004,31 @@
                 <a:rPr lang="en-GB" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>(∑▒〖</a:t>
+                <a:t>(∑</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="nl-NL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>▒</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>〖</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="nl-NL" sz="1100" b="0" i="0">
@@ -2022,7 +2048,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -2034,11 +2060,23 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t> −𝑥 ̅</a:t>
+                <a:t> −𝑥 ̅ )  ∗(𝑦 −𝑦 ̅)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>〗)/(∑</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="nl-NL" sz="1100" b="0" i="0">
@@ -2050,7 +2088,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t> )  (𝑦 −𝑦 ̅)</a:t>
+                <a:t>▒</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-GB" sz="1100" b="0" i="0">
@@ -2062,7 +2100,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>〗)/(∑▒〖</a:t>
+                <a:t>〖</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="nl-NL" sz="1100" b="0" i="0">
@@ -2092,8 +2130,8 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1543050" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -2226,7 +2264,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -2355,6 +2393,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2372,7 +2411,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2389,7 +2428,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2402,7 +2441,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2414,7 +2453,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2429,7 +2468,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -2442,7 +2481,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -2458,11 +2497,11 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
-                          <m:t> (</m:t>
+                          <m:t> ∗ (</m:t>
                         </m:r>
                         <m:r>
                           <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
@@ -2470,7 +2509,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2482,7 +2521,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2497,7 +2536,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2510,7 +2549,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2524,7 +2563,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2582,13 +2621,14 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-GB" sz="1100" b="0" i="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -2600,7 +2640,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -2612,7 +2652,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -2624,7 +2664,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -2636,7 +2676,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -2648,11 +2688,11 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t> −𝑥 ̅ )  (𝑦 −𝑦 ̅)</a:t>
+                <a:t> −𝑥 ̅ )  ∗ (𝑦 −𝑦 ̅)</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-GB" sz="1100" b="0" i="0">
@@ -2660,7 +2700,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -2682,8 +2722,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1562100" cy="409920"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -2725,6 +2765,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2742,7 +2783,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2757,7 +2798,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2769,7 +2810,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2781,7 +2822,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2796,7 +2837,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2809,7 +2850,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2823,7 +2864,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="+mn-lt"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2839,7 +2880,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -2957,8 +2998,8 @@
       <xdr:rowOff>22828</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="165558" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -3000,6 +3041,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3039,7 +3081,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -3097,10 +3139,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1562100" cy="172227"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3118,7 +3160,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="9991725" y="7067550"/>
+              <a:off x="9677400" y="7077075"/>
               <a:ext cx="1562100" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3147,177 +3189,197 @@
             <a:lstStyle/>
             <a:p>
               <a14:m>
-                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:sSub>
-                    <m:sSubPr>
-                      <m:ctrlPr>
-                        <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
-                          <a:solidFill>
-                            <a:schemeClr val="tx1"/>
-                          </a:solidFill>
-                          <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
-                          <a:ea typeface="+mn-ea"/>
-                          <a:cs typeface="+mn-cs"/>
-                        </a:rPr>
-                      </m:ctrlPr>
-                    </m:sSubPr>
-                    <m:e>
-                      <m:acc>
-                        <m:accPr>
-                          <m:chr m:val="̅"/>
-                          <m:ctrlPr>
-                            <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
-                              <a:solidFill>
-                                <a:schemeClr val="tx1"/>
-                              </a:solidFill>
-                              <a:effectLst/>
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              <a:ea typeface="+mn-ea"/>
-                              <a:cs typeface="+mn-cs"/>
-                            </a:rPr>
-                          </m:ctrlPr>
-                        </m:accPr>
-                        <m:e>
-                          <m:r>
-                            <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
-                              <a:solidFill>
-                                <a:schemeClr val="tx1"/>
-                              </a:solidFill>
-                              <a:effectLst/>
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              <a:ea typeface="+mn-ea"/>
-                              <a:cs typeface="+mn-cs"/>
-                            </a:rPr>
-                            <m:t>𝑦</m:t>
-                          </m:r>
-                        </m:e>
-                      </m:acc>
-                      <m:r>
-                        <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
-                          <a:solidFill>
-                            <a:schemeClr val="tx1"/>
-                          </a:solidFill>
-                          <a:effectLst/>
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="+mn-ea"/>
-                          <a:cs typeface="+mn-cs"/>
-                        </a:rPr>
-                        <m:t>=</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
-                          <a:solidFill>
-                            <a:schemeClr val="tx1"/>
-                          </a:solidFill>
-                          <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
-                          <a:ea typeface="+mn-ea"/>
-                          <a:cs typeface="+mn-cs"/>
-                        </a:rPr>
-                        <m:t>𝑏</m:t>
-                      </m:r>
-                    </m:e>
-                    <m:sub>
-                      <m:r>
-                        <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
-                          <a:solidFill>
-                            <a:schemeClr val="tx1"/>
-                          </a:solidFill>
-                          <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
-                          <a:ea typeface="+mn-ea"/>
-                          <a:cs typeface="+mn-cs"/>
-                        </a:rPr>
-                        <m:t>0</m:t>
-                      </m:r>
-                    </m:sub>
-                  </m:sSub>
-                  <m:r>
-                    <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1"/>
-                      </a:solidFill>
-                      <a:effectLst/>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:rPr>
-                    <m:t>+</m:t>
-                  </m:r>
-                  <m:sSub>
-                    <m:sSubPr>
-                      <m:ctrlPr>
-                        <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
-                          <a:solidFill>
-                            <a:schemeClr val="tx1"/>
-                          </a:solidFill>
-                          <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
-                          <a:ea typeface="+mn-ea"/>
-                          <a:cs typeface="+mn-cs"/>
-                        </a:rPr>
-                      </m:ctrlPr>
-                    </m:sSubPr>
-                    <m:e>
-                      <m:r>
-                        <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
-                          <a:solidFill>
-                            <a:schemeClr val="tx1"/>
-                          </a:solidFill>
-                          <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
-                          <a:ea typeface="+mn-ea"/>
-                          <a:cs typeface="+mn-cs"/>
-                        </a:rPr>
-                        <m:t>𝑏</m:t>
-                      </m:r>
-                    </m:e>
-                    <m:sub>
-                      <m:r>
-                        <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
-                          <a:solidFill>
-                            <a:schemeClr val="tx1"/>
-                          </a:solidFill>
-                          <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
-                          <a:ea typeface="+mn-ea"/>
-                          <a:cs typeface="+mn-cs"/>
-                        </a:rPr>
-                        <m:t>1</m:t>
-                      </m:r>
-                    </m:sub>
-                  </m:sSub>
-                  <m:r>
-                    <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1"/>
-                      </a:solidFill>
-                      <a:effectLst/>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:rPr>
-                    <m:t>∗</m:t>
-                  </m:r>
-                  <m:r>
-                    <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1"/>
-                      </a:solidFill>
-                      <a:effectLst/>
-                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:rPr>
-                    <m:t>𝑥</m:t>
-                  </m:r>
-                </m:oMath>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:acc>
+                          <m:accPr>
+                            <m:chr m:val="̅"/>
+                            <m:ctrlPr>
+                              <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:accPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑦</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:acc>
+                        <m:r>
+                          <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>=</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑏</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>0</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑏</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>∗</m:t>
+                    </m:r>
+                    <m:acc>
+                      <m:accPr>
+                        <m:chr m:val="̅"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:accPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="nl-NL" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:acc>
+                  </m:oMath>
+                </m:oMathPara>
               </a14:m>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100"/>
-                <a:t> </a:t>
-              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -3336,7 +3398,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="9991725" y="7067550"/>
+              <a:off x="9677400" y="7077075"/>
               <a:ext cx="1562100" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3370,52 +3432,13 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>〖</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="nl-NL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>𝑦 ̅=</a:t>
+                <a:t>〖𝑦 ̅=𝑏〗_0+𝑏_1∗𝑥 ̅</a:t>
               </a:r>
-              <a:r>
-                <a:rPr lang="nl-NL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝑏〗_0+𝑏_1∗</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="nl-NL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝑥</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100"/>
-                <a:t> </a:t>
-              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -3726,7 +3749,7 @@
   <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3765,235 +3788,235 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <f ca="1">RANDBETWEEN(60,200)</f>
-        <v>198</v>
+        <v>167</v>
       </c>
       <c r="B2">
         <f ca="1">(A2*0.8)+RANDBETWEEN(-8,8)</f>
-        <v>155.4</v>
+        <v>129.6</v>
       </c>
       <c r="C2" s="4">
-        <f ca="1">SUM(A2-$J$26)</f>
-        <v>52</v>
+        <f t="shared" ref="C2:C10" ca="1" si="0">SUM(A2-$J$26)</f>
+        <v>17.222222222222229</v>
       </c>
       <c r="D2" s="4">
-        <f ca="1">SUM(B2-$J$27)</f>
-        <v>40.488888888888894</v>
+        <f t="shared" ref="D2:D10" ca="1" si="1">SUM(B2-$J$27)</f>
+        <v>11.8888888888889</v>
       </c>
       <c r="E2" s="4">
-        <f ca="1">POWER(SUM(A2-$J$26), 2)</f>
-        <v>2704</v>
+        <f t="shared" ref="E2:E10" ca="1" si="2">POWER(SUM(A2-$J$26), 2)</f>
+        <v>296.60493827160514</v>
       </c>
       <c r="F2" s="4">
         <f ca="1">SUM(C2) * D2</f>
-        <v>2105.4222222222224</v>
+        <v>204.75308641975334</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ref="A3:A66" ca="1" si="0">RANDBETWEEN(60,200)</f>
-        <v>164</v>
+        <f t="shared" ref="A3:A10" ca="1" si="3">RANDBETWEEN(60,200)</f>
+        <v>149</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B66" ca="1" si="1">(A3*0.8)+RANDBETWEEN(-8,8)</f>
-        <v>127.20000000000002</v>
+        <f t="shared" ref="B3:B10" ca="1" si="4">(A3*0.8)+RANDBETWEEN(-8,8)</f>
+        <v>111.2</v>
       </c>
       <c r="C3" s="4">
-        <f ca="1">SUM(A3-$J$26)</f>
-        <v>18</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.77777777777777146</v>
       </c>
       <c r="D3" s="4">
-        <f ca="1">SUM(B3-$J$27)</f>
-        <v>12.288888888888906</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>-6.5111111111110915</v>
       </c>
       <c r="E3" s="4">
-        <f ca="1">POWER(SUM(A3-$J$26), 2)</f>
-        <v>324</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.60493827160492841</v>
       </c>
       <c r="F3" s="4">
-        <f t="shared" ref="F3:F66" ca="1" si="2">SUM(C3) * D3</f>
-        <v>221.2000000000003</v>
+        <f t="shared" ref="F3:F10" ca="1" si="5">SUM(C3) * D3</f>
+        <v>5.0641975308641412</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
+        <f t="shared" ca="1" si="3"/>
+        <v>116</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="4"/>
+        <v>94.800000000000011</v>
+      </c>
+      <c r="C4" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>129</v>
-      </c>
-      <c r="B4">
+        <v>-33.777777777777771</v>
+      </c>
+      <c r="D4" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>108.2</v>
-      </c>
-      <c r="C4" s="4">
-        <f ca="1">SUM(A4-$J$26)</f>
-        <v>-17</v>
-      </c>
-      <c r="D4" s="4">
-        <f ca="1">SUM(B4-$J$27)</f>
-        <v>-6.7111111111111086</v>
+        <v>-22.911111111111083</v>
       </c>
       <c r="E4" s="4">
-        <f ca="1">POWER(SUM(A4-$J$26), 2)</f>
-        <v>289</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1140.9382716049379</v>
       </c>
       <c r="F4" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>114.08888888888885</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>773.88641975308531</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
+        <f t="shared" ca="1" si="3"/>
+        <v>198</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="4"/>
+        <v>153.4</v>
+      </c>
+      <c r="C5" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
-      </c>
-      <c r="B5">
+        <v>48.222222222222229</v>
+      </c>
+      <c r="D5" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>63</v>
-      </c>
-      <c r="C5" s="4">
-        <f ca="1">SUM(A5-$J$26)</f>
-        <v>-61</v>
-      </c>
-      <c r="D5" s="4">
-        <f ca="1">SUM(B5-$J$27)</f>
-        <v>-51.911111111111111</v>
+        <v>35.688888888888911</v>
       </c>
       <c r="E5" s="4">
-        <f ca="1">POWER(SUM(A5-$J$26), 2)</f>
-        <v>3721</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>2325.3827160493834</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>3166.577777777778</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1720.9975308641988</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
+        <f t="shared" ca="1" si="3"/>
+        <v>153</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ca="1" si="4"/>
+        <v>125.4</v>
+      </c>
+      <c r="C6" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
-      </c>
-      <c r="B6">
+        <v>3.2222222222222285</v>
+      </c>
+      <c r="D6" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>57.600000000000009</v>
-      </c>
-      <c r="C6" s="4">
-        <f ca="1">SUM(A6-$J$26)</f>
-        <v>-64</v>
-      </c>
-      <c r="D6" s="4">
-        <f ca="1">SUM(B6-$J$27)</f>
-        <v>-57.311111111111103</v>
+        <v>7.6888888888889113</v>
       </c>
       <c r="E6" s="4">
-        <f ca="1">POWER(SUM(A6-$J$26), 2)</f>
-        <v>4096</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>10.382716049382756</v>
       </c>
       <c r="F6" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>3667.9111111111106</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>24.775308641975428</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
+        <f t="shared" ca="1" si="3"/>
+        <v>168</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ca="1" si="4"/>
+        <v>126.4</v>
+      </c>
+      <c r="C7" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>145</v>
-      </c>
-      <c r="B7">
+        <v>18.222222222222229</v>
+      </c>
+      <c r="D7" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>124</v>
-      </c>
-      <c r="C7" s="4">
-        <f ca="1">SUM(A7-$J$26)</f>
-        <v>-1</v>
-      </c>
-      <c r="D7" s="4">
-        <f ca="1">SUM(B7-$J$27)</f>
-        <v>9.0888888888888886</v>
+        <v>8.6888888888889113</v>
       </c>
       <c r="E7" s="4">
-        <f ca="1">POWER(SUM(A7-$J$26), 2)</f>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>332.04938271604959</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>-9.0888888888888886</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>158.33086419753133</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
+        <f t="shared" ca="1" si="3"/>
+        <v>198</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ca="1" si="4"/>
+        <v>163.4</v>
+      </c>
+      <c r="C8" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>196</v>
-      </c>
-      <c r="B8">
+        <v>48.222222222222229</v>
+      </c>
+      <c r="D8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>151.80000000000001</v>
-      </c>
-      <c r="C8" s="4">
-        <f ca="1">SUM(A8-$J$26)</f>
-        <v>50</v>
-      </c>
-      <c r="D8" s="4">
-        <f ca="1">SUM(B8-$J$27)</f>
-        <v>36.8888888888889</v>
+        <v>45.688888888888911</v>
       </c>
       <c r="E8" s="4">
-        <f ca="1">POWER(SUM(A8-$J$26), 2)</f>
-        <v>2500</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>2325.3827160493834</v>
       </c>
       <c r="F8" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>1844.444444444445</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2203.219753086421</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
+        <f t="shared" ca="1" si="3"/>
+        <v>67</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ca="1" si="4"/>
+        <v>48.6</v>
+      </c>
+      <c r="C9" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>193</v>
-      </c>
-      <c r="B9">
+        <v>-82.777777777777771</v>
+      </c>
+      <c r="D9" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>152.4</v>
-      </c>
-      <c r="C9" s="4">
-        <f ca="1">SUM(A9-$J$26)</f>
-        <v>47</v>
-      </c>
-      <c r="D9" s="4">
-        <f ca="1">SUM(B9-$J$27)</f>
-        <v>37.488888888888894</v>
+        <v>-69.111111111111086</v>
       </c>
       <c r="E9" s="4">
-        <f ca="1">POWER(SUM(A9-$J$26), 2)</f>
-        <v>2209</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>6852.1604938271594</v>
       </c>
       <c r="F9" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>1761.9777777777781</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>5720.8641975308619</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
+        <f t="shared" ca="1" si="3"/>
+        <v>132</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ca="1" si="4"/>
+        <v>106.60000000000001</v>
+      </c>
+      <c r="C10" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>122</v>
-      </c>
-      <c r="B10">
+        <v>-17.777777777777771</v>
+      </c>
+      <c r="D10" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>94.600000000000009</v>
-      </c>
-      <c r="C10" s="4">
-        <f ca="1">SUM(A10-$J$26)</f>
-        <v>-24</v>
-      </c>
-      <c r="D10" s="4">
-        <f ca="1">SUM(B10-$J$27)</f>
-        <v>-20.311111111111103</v>
+        <v>-11.111111111111086</v>
       </c>
       <c r="E10" s="4">
-        <f ca="1">POWER(SUM(A10-$J$26), 2)</f>
-        <v>576</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>316.04938271604914</v>
       </c>
       <c r="F10" s="4">
-        <f t="shared" ca="1" si="2"/>
-        <v>487.46666666666647</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>197.53086419753035</v>
       </c>
     </row>
     <row r="17" spans="9:12" x14ac:dyDescent="0.25">
@@ -4031,7 +4054,7 @@
       </c>
       <c r="J26">
         <f ca="1">AVERAGE(A2:A300)</f>
-        <v>146</v>
+        <v>149.77777777777777</v>
       </c>
     </row>
     <row r="27" spans="9:12" x14ac:dyDescent="0.25">
@@ -4040,7 +4063,7 @@
       </c>
       <c r="J27">
         <f ca="1">AVERAGE(B2:B300)</f>
-        <v>114.91111111111111</v>
+        <v>117.71111111111109</v>
       </c>
     </row>
     <row r="28" spans="9:12" x14ac:dyDescent="0.25">
@@ -4054,7 +4077,7 @@
       </c>
       <c r="L30">
         <f ca="1">SUM(F2:F301)</f>
-        <v>13360.000000000002</v>
+        <v>11009.422222222222</v>
       </c>
     </row>
     <row r="31" spans="9:12" x14ac:dyDescent="0.25">
@@ -4068,7 +4091,7 @@
       </c>
       <c r="L33">
         <f ca="1">SUM(E2:E301)</f>
-        <v>16420</v>
+        <v>13599.555555555557</v>
       </c>
     </row>
     <row r="34" spans="9:15" x14ac:dyDescent="0.25">
@@ -4082,7 +4105,7 @@
       </c>
       <c r="L35">
         <f ca="1">L30/L33</f>
-        <v>0.81364190012180282</v>
+        <v>0.80954279551619324</v>
       </c>
     </row>
     <row r="37" spans="9:15" x14ac:dyDescent="0.25">
@@ -4093,7 +4116,7 @@
     <row r="39" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I39">
         <f ca="1">J27</f>
-        <v>114.91111111111111</v>
+        <v>117.71111111111109</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>10</v>
@@ -4106,20 +4129,20 @@
       </c>
       <c r="M39">
         <f ca="1">L35</f>
-        <v>0.81364190012180282</v>
+        <v>0.80954279551619324</v>
       </c>
       <c r="N39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="O39">
         <f ca="1">J26</f>
-        <v>146</v>
+        <v>149.77777777777777</v>
       </c>
     </row>
     <row r="40" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I40">
         <f ca="1">J27</f>
-        <v>114.91111111111111</v>
+        <v>117.71111111111109</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>10</v>
@@ -4132,13 +4155,13 @@
       </c>
       <c r="M40">
         <f ca="1">SUM(M39*O39)</f>
-        <v>118.79171741778322</v>
+        <v>121.25152092842538</v>
       </c>
     </row>
     <row r="41" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I41">
         <f ca="1">SUM(I40-M40)</f>
-        <v>-3.8806063066721066</v>
+        <v>-3.5404098173142842</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>10</v>
@@ -4170,7 +4193,7 @@
     <row r="47" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I47" s="3">
         <f ca="1">SUM(I41+L35*I45)</f>
-        <v>138.50672621464338</v>
+        <v>138.12957939801953</v>
       </c>
     </row>
   </sheetData>

</xml_diff>